<commit_message>
add to upload to excel sheet
</commit_message>
<xml_diff>
--- a/Flat.File.ShippingConfirm (1).xlsx
+++ b/Flat.File.ShippingConfirm (1).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3270" yWindow="2550" windowWidth="21600" windowHeight="11295" tabRatio="716" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5940" yWindow="1500" windowWidth="21600" windowHeight="11295" tabRatio="716" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Definitions" sheetId="1" state="visible" r:id="rId1"/>
@@ -351,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -471,6 +471,9 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -490,10 +493,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -906,15 +905,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col width="34.42578125" customWidth="1" style="53" min="1" max="1"/>
-    <col width="83.85546875" customWidth="1" style="53" min="2" max="2"/>
-    <col width="53.85546875" customWidth="1" style="54" min="3" max="3"/>
-    <col width="39.85546875" customWidth="1" style="53" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="53" min="5" max="257"/>
+    <col width="34.42578125" customWidth="1" style="52" min="1" max="1"/>
+    <col width="83.85546875" customWidth="1" style="52" min="2" max="2"/>
+    <col width="53.85546875" customWidth="1" style="53" min="3" max="3"/>
+    <col width="39.85546875" customWidth="1" style="52" min="4" max="4"/>
+    <col width="9.140625" customWidth="1" style="52" min="5" max="257"/>
   </cols>
   <sheetData>
     <row r="1" ht="30.95" customHeight="1">
-      <c r="A1" s="52" t="inlineStr">
+      <c r="A1" s="51" t="inlineStr">
         <is>
           <t>Definitions - Shipping Confirmation Template</t>
         </is>
@@ -1378,10 +1377,10 @@
       <c r="I22" s="32" t="n"/>
     </row>
     <row r="23" ht="15.6" customFormat="1" customHeight="1" s="33">
-      <c r="A23" s="44" t="n"/>
-      <c r="B23" s="44" t="n"/>
-      <c r="C23" s="45" t="n"/>
-      <c r="D23" s="46" t="n"/>
+      <c r="A23" s="45" t="n"/>
+      <c r="B23" s="45" t="n"/>
+      <c r="C23" s="46" t="n"/>
+      <c r="D23" s="47" t="n"/>
     </row>
     <row r="24" ht="12.95" customFormat="1" customHeight="1" s="13">
       <c r="A24" s="33" t="inlineStr">
@@ -1437,24 +1436,24 @@
       <c r="D29" s="38" t="n"/>
     </row>
     <row r="30" ht="13.15" customHeight="1">
-      <c r="A30" s="60" t="inlineStr">
+      <c r="A30" s="59" t="inlineStr">
         <is>
           <t xml:space="preserve">If you are shipping to specific countries where Amazon is responsible under local regulations to remit taxes on sales by selling partners, the tax collection model may be determined by the ship from address that you enter.  Hence, please provide the ship-from-address based on the actual address from where the item was shipped.   If you do not provide a ship from address , Amazon will assume the default ship from location that you provided in your Seller Central account shipping settings/template" at the time when the order was placed.  </t>
         </is>
       </c>
-      <c r="B30" s="56" t="n"/>
-      <c r="C30" s="56" t="n"/>
-      <c r="D30" s="57" t="n"/>
+      <c r="B30" s="55" t="n"/>
+      <c r="C30" s="55" t="n"/>
+      <c r="D30" s="56" t="n"/>
     </row>
     <row r="31" ht="12.95" customHeight="1">
-      <c r="A31" s="55" t="inlineStr">
+      <c r="A31" s="54" t="inlineStr">
         <is>
           <t>If you have not shipped the order from the default warehouse location that is provided in your Seller Central account shipping settings/template" at the time when the order was placed, then this may impact the tax collection model for the order. For additional information, please visit the help page - https://sellercentral.amazon.com/gp/help/help.html?itemID=GSF678GXLDTTTETZ</t>
         </is>
       </c>
-      <c r="B31" s="56" t="n"/>
-      <c r="C31" s="56" t="n"/>
-      <c r="D31" s="57" t="n"/>
+      <c r="B31" s="55" t="n"/>
+      <c r="C31" s="55" t="n"/>
+      <c r="D31" s="56" t="n"/>
     </row>
     <row r="32" ht="13.35" customHeight="1">
       <c r="A32" s="39" t="n"/>
@@ -1463,7 +1462,7 @@
       <c r="D32" s="25" t="n"/>
     </row>
     <row r="33" ht="13.35" customHeight="1">
-      <c r="A33" s="47" t="inlineStr">
+      <c r="A33" s="48" t="inlineStr">
         <is>
           <t>Important Note regarding ship from address:</t>
         </is>
@@ -1473,44 +1472,44 @@
       <c r="D33" s="13" t="n"/>
     </row>
     <row r="34" ht="12.95" customHeight="1">
-      <c r="A34" s="59" t="inlineStr">
+      <c r="A34" s="58" t="inlineStr">
         <is>
           <t>If you are shipping to specific countries where Amazon is responsible under local regulations to remit taxes on sales by selling partners, the tax collection model may be determined by the ship from address that you enter. Hence, please provide the ship-from-address based on the actual address from where the item was shipped. If you do not provide a ship from address, Amazon will assume the default ship from location that you provided in your Seller Central account shipping settings/template" at the time when the order was placed. If you have S2ID (Supply Source ID) available through get S2 API or Locations tab under Shipping Settings on Seller Central, please share the S2ID during ship confirm. Supply Sources/Locations tab are currently available to Sellers operating in US. Amazon will consider S2 ID as the primary input for ship from location, wherever available.</t>
         </is>
       </c>
-      <c r="B34" s="56" t="n"/>
-      <c r="C34" s="56" t="n"/>
-      <c r="D34" s="57" t="n"/>
+      <c r="B34" s="55" t="n"/>
+      <c r="C34" s="55" t="n"/>
+      <c r="D34" s="56" t="n"/>
     </row>
     <row r="35" ht="12.95" customHeight="1">
-      <c r="A35" s="48" t="inlineStr">
+      <c r="A35" s="49" t="inlineStr">
         <is>
           <t>To learn more about get S2 API. Click here.</t>
         </is>
       </c>
-      <c r="B35" s="59" t="n"/>
-      <c r="C35" s="59" t="n"/>
-      <c r="D35" s="59" t="n"/>
+      <c r="B35" s="58" t="n"/>
+      <c r="C35" s="58" t="n"/>
+      <c r="D35" s="58" t="n"/>
     </row>
     <row r="36" ht="12.95" customHeight="1">
-      <c r="A36" s="48" t="inlineStr">
+      <c r="A36" s="49" t="inlineStr">
         <is>
           <t>To learn more about Locations tab. Click here.</t>
         </is>
       </c>
-      <c r="B36" s="59" t="n"/>
-      <c r="C36" s="59" t="n"/>
-      <c r="D36" s="59" t="n"/>
+      <c r="B36" s="58" t="n"/>
+      <c r="C36" s="58" t="n"/>
+      <c r="D36" s="58" t="n"/>
     </row>
     <row r="37" ht="12.95" customHeight="1">
-      <c r="A37" s="58" t="inlineStr">
+      <c r="A37" s="57" t="inlineStr">
         <is>
           <t>If you have not shipped the order from the default warehouse location that is provided in your Seller Central account shipping settings/template" at the time when the order was placed, then this may impact the tax collection model for the order. For additional information, please visit the help page - https://sellercentral.amazon.com/gp/help/help.html?itemID=GSF678GXLDTTTETZ</t>
         </is>
       </c>
-      <c r="B37" s="56" t="n"/>
-      <c r="C37" s="56" t="n"/>
-      <c r="D37" s="57" t="n"/>
+      <c r="B37" s="55" t="n"/>
+      <c r="C37" s="55" t="n"/>
+      <c r="D37" s="56" t="n"/>
     </row>
     <row r="39" ht="12.95" customHeight="1">
       <c r="A39" s="37" t="inlineStr">
@@ -1523,14 +1522,14 @@
       <c r="D39" s="25" t="n"/>
     </row>
     <row r="40" ht="12.95" customHeight="1">
-      <c r="A40" s="55" t="inlineStr">
+      <c r="A40" s="54" t="inlineStr">
         <is>
           <t xml:space="preserve"> If you split an order into multiple shipments, all the shipments in the order must be shipped from the same country as the first shipment. For additional information, please visit this help page - https://sellercentral.amazon.com/gp/help/G641</t>
         </is>
       </c>
-      <c r="B40" s="56" t="n"/>
-      <c r="C40" s="56" t="n"/>
-      <c r="D40" s="57" t="n"/>
+      <c r="B40" s="55" t="n"/>
+      <c r="C40" s="55" t="n"/>
+      <c r="D40" s="56" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1566,36 +1565,38 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col width="26.85546875" customWidth="1" style="51" min="1" max="1"/>
-    <col width="11.85546875" bestFit="1" customWidth="1" style="41" min="2" max="2"/>
-    <col width="6.28515625" bestFit="1" customWidth="1" style="41" min="3" max="3"/>
-    <col width="7.28515625" bestFit="1" customWidth="1" style="41" min="4" max="5"/>
-    <col width="12.42578125" bestFit="1" customWidth="1" style="41" min="6" max="6"/>
-    <col width="7.7109375" bestFit="1" customWidth="1" style="41" min="7" max="7"/>
-    <col width="18.42578125" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="24.42578125" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="21.85546875" bestFit="1" customWidth="1" min="10" max="12"/>
-    <col width="22.7109375" bestFit="1" customWidth="1" min="13" max="13"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" min="14" max="14"/>
-    <col width="23.5703125" bestFit="1" customWidth="1" min="15" max="15"/>
-    <col width="22.7109375" bestFit="1" customWidth="1" min="16" max="16"/>
-    <col width="24" bestFit="1" customWidth="1" min="17" max="17"/>
-    <col width="16.42578125" bestFit="1" customWidth="1" min="18" max="18"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="41" min="1" max="1"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" style="41" min="2" max="2"/>
+    <col width="8" bestFit="1" customWidth="1" style="41" min="3" max="3"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="41" min="4" max="4"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" style="41" min="5" max="5"/>
+    <col width="7.28515625" bestFit="1" customWidth="1" style="41" min="6" max="6"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" style="41" min="7" max="7"/>
+    <col width="7.7109375" bestFit="1" customWidth="1" style="41" min="8" max="8"/>
+    <col width="18.42578125" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="24.42578125" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="21.85546875" bestFit="1" customWidth="1" min="11" max="13"/>
+    <col width="22.7109375" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="23.5703125" bestFit="1" customWidth="1" min="16" max="16"/>
+    <col width="22.7109375" bestFit="1" customWidth="1" min="17" max="17"/>
+    <col width="24" bestFit="1" customWidth="1" min="18" max="18"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.1" customHeight="1">
-      <c r="A1" s="50" t="inlineStr">
+      <c r="A1" s="42" t="inlineStr">
         <is>
           <t>order-id</t>
         </is>
@@ -1605,345 +1606,706 @@
           <t>order-item-id</t>
         </is>
       </c>
-      <c r="C1" s="42" t="inlineStr">
-        <is>
-          <t>new value</t>
-        </is>
-      </c>
-      <c r="D1" s="32" t="inlineStr">
+      <c r="C1" s="43" t="inlineStr">
+        <is>
+          <t>quantity</t>
+        </is>
+      </c>
+      <c r="D1" s="42" t="inlineStr">
+        <is>
+          <t>ship-date</t>
+        </is>
+      </c>
+      <c r="E1" s="32" t="inlineStr">
         <is>
           <t>carrier-code</t>
         </is>
       </c>
-      <c r="E1" s="32" t="inlineStr">
+      <c r="F1" s="32" t="inlineStr">
         <is>
           <t>carrier-name</t>
         </is>
       </c>
-      <c r="F1" s="32" t="inlineStr">
+      <c r="G1" s="32" t="inlineStr">
         <is>
           <t>tracking-number</t>
         </is>
       </c>
-      <c r="G1" s="32" t="inlineStr">
+      <c r="H1" s="32" t="inlineStr">
         <is>
           <t>ship-method</t>
         </is>
       </c>
-      <c r="H1" s="43" t="inlineStr">
+      <c r="I1" s="44" t="inlineStr">
         <is>
           <t>transparency_code</t>
         </is>
       </c>
-      <c r="I1" s="43" t="inlineStr">
+      <c r="J1" s="44" t="inlineStr">
         <is>
           <t>ship_from_address_name</t>
         </is>
       </c>
-      <c r="J1" s="43" t="inlineStr">
+      <c r="K1" s="44" t="inlineStr">
         <is>
           <t>ship_from_address_line1</t>
         </is>
       </c>
-      <c r="K1" s="43" t="inlineStr">
+      <c r="L1" s="44" t="inlineStr">
         <is>
           <t>ship_from_address_line2</t>
         </is>
       </c>
-      <c r="L1" s="43" t="inlineStr">
+      <c r="M1" s="44" t="inlineStr">
         <is>
           <t>ship_from_address_line3</t>
         </is>
       </c>
-      <c r="M1" s="43" t="inlineStr">
+      <c r="N1" s="44" t="inlineStr">
         <is>
           <t>ship_from_address_city</t>
         </is>
       </c>
-      <c r="N1" s="43" t="inlineStr">
+      <c r="O1" s="44" t="inlineStr">
         <is>
           <t>ship_from_address_county</t>
         </is>
       </c>
-      <c r="O1" s="43" t="inlineStr">
+      <c r="P1" s="44" t="inlineStr">
         <is>
           <t>ship_from_address_state_or_region</t>
         </is>
       </c>
-      <c r="P1" s="43" t="inlineStr">
+      <c r="Q1" s="44" t="inlineStr">
         <is>
           <t>ship_from_address_postalcode</t>
         </is>
       </c>
-      <c r="Q1" s="43" t="inlineStr">
+      <c r="R1" s="44" t="inlineStr">
         <is>
           <t>ship_from_address_countrycode</t>
         </is>
       </c>
-      <c r="R1" s="43" t="inlineStr">
+      <c r="S1" s="44" t="inlineStr">
         <is>
           <t>ship_from_supply_source_id</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>67847346292349</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>112-0739580-2127405</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>01-12943-02622</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>634926538593480</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00773958</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>67847346292359</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>112-9097798-1337002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>08-12934-05272</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>634926538593490</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00774920</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>67847346292369</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>111-3312612-3798619</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10-12931-53185</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>634926538593500</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00774948</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>67847346292379</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>112-6459511-0925003</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>22-12917-11654</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>634926538593510</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00776599</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>67847346292389</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>114-2428484-4385809</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>08-12933-67589</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>634926538593520</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33342778</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>67847346292399</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>113-8231624-4633820</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>07-12934-88562</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>634926538593530</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33352525</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>67847346292409</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>114-9501012-9881065</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>702945401</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>634926538593540</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1ZA5T3520301375646</t>
+        </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>67847346292419</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>111-2116348-3772222</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>12-12929-22125</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F9" t="n">
-        <v>634926538593550</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33355460</t>
+        </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>67847346292429</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>114-2562213-5284212</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13-12927-84015</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>634926538593560</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1Z8126VR0333346101</t>
+        </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>67847346292439</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>111-1894995-3969806</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>23-12915-55552</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>634926538593570</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01389964</t>
+        </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>67847346292349</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>112-3822813-0294626</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>703189906</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>634926538593480</v>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00777123</t>
+        </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>67847346292359</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>114-8958109-1982618</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>703206280</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F13" t="n">
-        <v>634926538593490</v>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1Z3024W20200778104</t>
+        </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>67847346292369</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>114-3603849-6770617</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06-12936-50217</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F14" t="n">
-        <v>634926538593500</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33353935</t>
+        </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>67847346292379</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>114-6687719-7177854</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>25-12913-69501</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F15" t="n">
-        <v>634926538593510</v>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33360696</t>
+        </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>67847346292389</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>113-6431855-1707410</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>702917227</t>
+        </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F16" t="n">
-        <v>634926538593520</v>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33342223</t>
+        </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>67847346292399</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>111-4196409-3211422</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>07-12931-74346</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F17" t="n">
-        <v>634926538593530</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33285947</t>
+        </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>67847346292409</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>112-3616143-6610663</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>14-12923-67816</t>
+        </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F18" t="n">
-        <v>634926538593540</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33280602</t>
+        </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>67847346292419</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>112-2803937-5654632</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>702914437</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F19" t="n">
-        <v>634926538593550</v>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33352374</t>
+        </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>67847346292429</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>113-6413731-1090631</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>702942056</t>
+        </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F20" t="n">
-        <v>634926538593560</v>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>9234690185108900016648</t>
+        </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>67847346292439</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>111-5534447-2556238</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>02-12942-39922</t>
+        </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="F21" t="n">
-        <v>634926538593570</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01399846</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>112-1404559-5127409</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>07-12935-80266</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01398936</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>111-9945324-9853836</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>703212138</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1ZA5T3520201400315</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>114-8327013-2852237</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>10-12931-62213</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01397384</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>114-2733954-5928252</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>703195679</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1ZA5T3520201399944</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>111-1960000-7331436</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>703042547</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01397982</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>113-1778148-4749838</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>01-12947-15133</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00802738</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>114-3140840-2805024</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>15-12928-93200</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1ZA5T3520301443287</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>112-0163782-4789872</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>18-12925-65132</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>1Z3024W20300799170</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add file paths to enviroment variables and trash messages that have match in tsv file
</commit_message>
<xml_diff>
--- a/Flat.File.ShippingConfirm (1).xlsx
+++ b/Flat.File.ShippingConfirm (1).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5940" yWindow="1500" windowWidth="21600" windowHeight="11295" tabRatio="716" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="716" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Definitions" sheetId="1" state="visible" r:id="rId1"/>
@@ -903,16 +903,16 @@
       <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col width="34.42578125" customWidth="1" style="52" min="1" max="1"/>
-    <col width="83.85546875" customWidth="1" style="52" min="2" max="2"/>
-    <col width="53.85546875" customWidth="1" style="53" min="3" max="3"/>
-    <col width="39.85546875" customWidth="1" style="52" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="52" min="5" max="257"/>
+    <col width="34.44140625" customWidth="1" style="52" min="1" max="1"/>
+    <col width="83.88671875" customWidth="1" style="52" min="2" max="2"/>
+    <col width="53.88671875" customWidth="1" style="53" min="3" max="3"/>
+    <col width="39.88671875" customWidth="1" style="52" min="4" max="4"/>
+    <col width="9.109375" customWidth="1" style="52" min="5" max="257"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30.95" customHeight="1">
+    <row r="1" ht="30.9" customHeight="1">
       <c r="A1" s="51" t="inlineStr">
         <is>
           <t>Definitions - Shipping Confirmation Template</t>
@@ -928,7 +928,7 @@
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="4" t="n"/>
     </row>
-    <row r="3" ht="12.95" customFormat="1" customHeight="1" s="6">
+    <row r="3" ht="12.9" customFormat="1" customHeight="1" s="6">
       <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Label Name</t>
@@ -950,7 +950,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="24.95" customHeight="1">
+    <row r="4" ht="24.9" customHeight="1">
       <c r="A4" s="7" t="inlineStr">
         <is>
           <t>order-id</t>
@@ -972,7 +972,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="38.45" customHeight="1">
+    <row r="5" ht="38.4" customHeight="1">
       <c r="A5" s="11" t="inlineStr">
         <is>
           <t>order-item-id</t>
@@ -1037,7 +1037,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" ht="137.45" customHeight="1">
+    <row r="8" ht="137.4" customHeight="1">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>carrier-code</t>
@@ -1060,7 +1060,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="24.95" customHeight="1">
+    <row r="9" ht="24.9" customHeight="1">
       <c r="A9" s="11" t="inlineStr">
         <is>
           <t>carrier-name</t>
@@ -1083,7 +1083,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="24.95" customHeight="1">
+    <row r="10" ht="24.9" customHeight="1">
       <c r="A10" s="11" t="inlineStr">
         <is>
           <t>tracking-number</t>
@@ -1104,7 +1104,7 @@
         <v>22344455</v>
       </c>
     </row>
-    <row r="11" ht="24.95" customHeight="1">
+    <row r="11" ht="24.9" customHeight="1">
       <c r="A11" s="13" t="inlineStr">
         <is>
           <t>ship-method</t>
@@ -1148,7 +1148,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="24.95" customFormat="1" customHeight="1" s="13">
+    <row r="13" ht="24.9" customFormat="1" customHeight="1" s="13">
       <c r="A13" s="11" t="inlineStr">
         <is>
           <t>ship_from_address_name</t>
@@ -1170,7 +1170,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="12.95" customFormat="1" customHeight="1" s="13">
+    <row r="14" ht="12.9" customFormat="1" customHeight="1" s="13">
       <c r="A14" s="20" t="inlineStr">
         <is>
           <t>ship_from_address_line1</t>
@@ -1192,7 +1192,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="12.95" customFormat="1" customHeight="1" s="13">
+    <row r="15" ht="12.9" customFormat="1" customHeight="1" s="13">
       <c r="A15" s="24" t="inlineStr">
         <is>
           <t>ship_from_address_line2</t>
@@ -1214,7 +1214,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="12.95" customFormat="1" customHeight="1" s="13">
+    <row r="16" ht="12.9" customFormat="1" customHeight="1" s="13">
       <c r="A16" s="24" t="inlineStr">
         <is>
           <t>ship_from_address_line3</t>
@@ -1236,7 +1236,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="12.95" customFormat="1" customHeight="1" s="13">
+    <row r="17" ht="12.9" customFormat="1" customHeight="1" s="13">
       <c r="A17" s="24" t="inlineStr">
         <is>
           <t>ship_from_address_city</t>
@@ -1258,7 +1258,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="12.95" customFormat="1" customHeight="1" s="13">
+    <row r="18" ht="12.9" customFormat="1" customHeight="1" s="13">
       <c r="A18" s="24" t="inlineStr">
         <is>
           <t>ship_from_address_county</t>
@@ -1280,7 +1280,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="12.95" customFormat="1" customHeight="1" s="13">
+    <row r="19" ht="12.9" customFormat="1" customHeight="1" s="13">
       <c r="A19" s="24" t="inlineStr">
         <is>
           <t>ship_from_address_state_or_region</t>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="12.95" customFormat="1" customHeight="1" s="13">
+    <row r="20" ht="12.9" customFormat="1" customHeight="1" s="13">
       <c r="A20" s="24" t="inlineStr">
         <is>
           <t>ship_from_address_postalcode</t>
@@ -1322,7 +1322,7 @@
         <v>32091</v>
       </c>
     </row>
-    <row r="21" ht="12.95" customFormat="1" customHeight="1" s="13">
+    <row r="21" ht="12.9" customFormat="1" customHeight="1" s="13">
       <c r="A21" s="30" t="inlineStr">
         <is>
           <t>ship_from_address_countrycode</t>
@@ -1349,7 +1349,7 @@
       <c r="H21" s="32" t="n"/>
       <c r="I21" s="32" t="n"/>
     </row>
-    <row r="22" ht="12.95" customFormat="1" customHeight="1" s="13">
+    <row r="22" ht="12.9" customFormat="1" customHeight="1" s="13">
       <c r="A22" s="30" t="inlineStr">
         <is>
           <t>ship_from_supply_source_id</t>
@@ -1382,7 +1382,7 @@
       <c r="C23" s="46" t="n"/>
       <c r="D23" s="47" t="n"/>
     </row>
-    <row r="24" ht="12.95" customFormat="1" customHeight="1" s="13">
+    <row r="24" ht="12.9" customFormat="1" customHeight="1" s="13">
       <c r="A24" s="33" t="inlineStr">
         <is>
           <t>Important Note Regarding Split Shipments and Transparency:</t>
@@ -1392,14 +1392,14 @@
       <c r="C24" s="33" t="n"/>
       <c r="D24" s="33" t="n"/>
     </row>
-    <row r="25" ht="15.95" customFormat="1" customHeight="1" s="13">
+    <row r="25" ht="15.9" customFormat="1" customHeight="1" s="13">
       <c r="A25" s="13" t="inlineStr">
         <is>
           <t>If a customer has ordered more than one item from you, and you are fulfilling the order in more than one shipment, then order-id, order-item-id, quantity and ship-date are all required for each shipment that you are confirming.</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="13.15" customHeight="1">
+    <row r="26" ht="13.2" customHeight="1">
       <c r="A26" s="33" t="inlineStr">
         <is>
           <t>If a product is enrolled in Transparency, you are required to send Transparency codes at ship confirmation, and order-id, order-item-id, quantity, ship-date and Transparency codes are all required.</t>
@@ -1409,7 +1409,7 @@
       <c r="C26" s="33" t="n"/>
       <c r="D26" s="33" t="n"/>
     </row>
-    <row r="27" ht="12.95" customHeight="1">
+    <row r="27" ht="12.9" customHeight="1">
       <c r="A27" s="34" t="inlineStr">
         <is>
           <t>To learn more about Transparency. Click here.</t>
@@ -1425,7 +1425,7 @@
       <c r="C28" s="36" t="n"/>
       <c r="D28" s="35" t="n"/>
     </row>
-    <row r="29" ht="12.95" customHeight="1">
+    <row r="29" ht="12.9" customHeight="1">
       <c r="A29" s="37" t="inlineStr">
         <is>
           <t>Important Note regarding ship from address:</t>
@@ -1435,7 +1435,7 @@
       <c r="C29" s="38" t="n"/>
       <c r="D29" s="38" t="n"/>
     </row>
-    <row r="30" ht="13.15" customHeight="1">
+    <row r="30" ht="13.2" customHeight="1">
       <c r="A30" s="59" t="inlineStr">
         <is>
           <t xml:space="preserve">If you are shipping to specific countries where Amazon is responsible under local regulations to remit taxes on sales by selling partners, the tax collection model may be determined by the ship from address that you enter.  Hence, please provide the ship-from-address based on the actual address from where the item was shipped.   If you do not provide a ship from address , Amazon will assume the default ship from location that you provided in your Seller Central account shipping settings/template" at the time when the order was placed.  </t>
@@ -1445,7 +1445,7 @@
       <c r="C30" s="55" t="n"/>
       <c r="D30" s="56" t="n"/>
     </row>
-    <row r="31" ht="12.95" customHeight="1">
+    <row r="31" ht="12.9" customHeight="1">
       <c r="A31" s="54" t="inlineStr">
         <is>
           <t>If you have not shipped the order from the default warehouse location that is provided in your Seller Central account shipping settings/template" at the time when the order was placed, then this may impact the tax collection model for the order. For additional information, please visit the help page - https://sellercentral.amazon.com/gp/help/help.html?itemID=GSF678GXLDTTTETZ</t>
@@ -1471,7 +1471,7 @@
       <c r="C33" s="13" t="n"/>
       <c r="D33" s="13" t="n"/>
     </row>
-    <row r="34" ht="12.95" customHeight="1">
+    <row r="34" ht="12.9" customHeight="1">
       <c r="A34" s="58" t="inlineStr">
         <is>
           <t>If you are shipping to specific countries where Amazon is responsible under local regulations to remit taxes on sales by selling partners, the tax collection model may be determined by the ship from address that you enter. Hence, please provide the ship-from-address based on the actual address from where the item was shipped. If you do not provide a ship from address, Amazon will assume the default ship from location that you provided in your Seller Central account shipping settings/template" at the time when the order was placed. If you have S2ID (Supply Source ID) available through get S2 API or Locations tab under Shipping Settings on Seller Central, please share the S2ID during ship confirm. Supply Sources/Locations tab are currently available to Sellers operating in US. Amazon will consider S2 ID as the primary input for ship from location, wherever available.</t>
@@ -1481,7 +1481,7 @@
       <c r="C34" s="55" t="n"/>
       <c r="D34" s="56" t="n"/>
     </row>
-    <row r="35" ht="12.95" customHeight="1">
+    <row r="35" ht="12.9" customHeight="1">
       <c r="A35" s="49" t="inlineStr">
         <is>
           <t>To learn more about get S2 API. Click here.</t>
@@ -1491,7 +1491,7 @@
       <c r="C35" s="58" t="n"/>
       <c r="D35" s="58" t="n"/>
     </row>
-    <row r="36" ht="12.95" customHeight="1">
+    <row r="36" ht="12.9" customHeight="1">
       <c r="A36" s="49" t="inlineStr">
         <is>
           <t>To learn more about Locations tab. Click here.</t>
@@ -1501,7 +1501,7 @@
       <c r="C36" s="58" t="n"/>
       <c r="D36" s="58" t="n"/>
     </row>
-    <row r="37" ht="12.95" customHeight="1">
+    <row r="37" ht="12.9" customHeight="1">
       <c r="A37" s="57" t="inlineStr">
         <is>
           <t>If you have not shipped the order from the default warehouse location that is provided in your Seller Central account shipping settings/template" at the time when the order was placed, then this may impact the tax collection model for the order. For additional information, please visit the help page - https://sellercentral.amazon.com/gp/help/help.html?itemID=GSF678GXLDTTTETZ</t>
@@ -1511,7 +1511,7 @@
       <c r="C37" s="55" t="n"/>
       <c r="D37" s="56" t="n"/>
     </row>
-    <row r="39" ht="12.95" customHeight="1">
+    <row r="39" ht="12.9" customHeight="1">
       <c r="A39" s="37" t="inlineStr">
         <is>
           <t>Important Note regarding orders split into multiple shipments</t>
@@ -1521,7 +1521,7 @@
       <c r="C39" s="25" t="n"/>
       <c r="D39" s="25" t="n"/>
     </row>
-    <row r="40" ht="12.95" customHeight="1">
+    <row r="40" ht="12.9" customHeight="1">
       <c r="A40" s="54" t="inlineStr">
         <is>
           <t xml:space="preserve"> If you split an order into multiple shipments, all the shipments in the order must be shipped from the same country as the first shipment. For additional information, please visit this help page - https://sellercentral.amazon.com/gp/help/G641</t>
@@ -1565,34 +1565,34 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I68" sqref="I68"/>
+      <selection pane="bottomRight" activeCell="A44" sqref="A2:XFD44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col width="19.42578125" bestFit="1" customWidth="1" style="41" min="1" max="1"/>
-    <col width="14.28515625" bestFit="1" customWidth="1" style="41" min="2" max="2"/>
+    <col width="19.44140625" bestFit="1" customWidth="1" style="41" min="1" max="1"/>
+    <col width="14.33203125" bestFit="1" customWidth="1" style="41" min="2" max="2"/>
     <col width="8" bestFit="1" customWidth="1" style="41" min="3" max="3"/>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="41" min="4" max="4"/>
-    <col width="23.42578125" bestFit="1" customWidth="1" style="41" min="5" max="5"/>
-    <col width="7.28515625" bestFit="1" customWidth="1" style="41" min="6" max="6"/>
-    <col width="23.42578125" bestFit="1" customWidth="1" style="41" min="7" max="7"/>
-    <col width="7.7109375" bestFit="1" customWidth="1" style="41" min="8" max="8"/>
-    <col width="18.42578125" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="24.42578125" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="21.85546875" bestFit="1" customWidth="1" min="11" max="13"/>
-    <col width="22.7109375" bestFit="1" customWidth="1" min="14" max="14"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" min="15" max="15"/>
-    <col width="23.5703125" bestFit="1" customWidth="1" min="16" max="16"/>
-    <col width="22.7109375" bestFit="1" customWidth="1" min="17" max="17"/>
+    <col width="5.88671875" bestFit="1" customWidth="1" style="41" min="4" max="4"/>
+    <col width="23.44140625" bestFit="1" customWidth="1" style="41" min="5" max="5"/>
+    <col width="7.33203125" bestFit="1" customWidth="1" style="41" min="6" max="6"/>
+    <col width="23.44140625" bestFit="1" customWidth="1" style="41" min="7" max="7"/>
+    <col width="7.6640625" bestFit="1" customWidth="1" style="41" min="8" max="8"/>
+    <col width="18.44140625" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="24.44140625" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="21.88671875" bestFit="1" customWidth="1" min="11" max="13"/>
+    <col width="22.6640625" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="21.6640625" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="23.5546875" bestFit="1" customWidth="1" min="16" max="16"/>
+    <col width="22.6640625" bestFit="1" customWidth="1" min="17" max="17"/>
     <col width="24" bestFit="1" customWidth="1" min="18" max="18"/>
-    <col width="16.42578125" bestFit="1" customWidth="1" min="19" max="19"/>
+    <col width="16.44140625" bestFit="1" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.1" customHeight="1">
@@ -2041,6 +2041,600 @@
       <c r="G17" t="inlineStr">
         <is>
           <t>1Z8126VRYW33285947</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>112-3616143-6610663</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>14-12923-67816</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33280602</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>112-2803937-5654632</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>702914437</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33352374</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>113-6413731-1090631</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>702942056</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>USPS</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>9234690185108900016648</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>111-5534447-2556238</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>02-12942-39922</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01399846</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>112-1404559-5127409</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>07-12935-80266</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01398936</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>111-9945324-9853836</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>703212138</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1ZA5T3520201400315</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>114-8327013-2852237</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>10-12931-62213</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01397384</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>114-2733954-5928252</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>703195679</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1ZA5T3520201399944</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>111-1960000-7331436</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>703042547</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01397982</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>113-1778148-4749838</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>01-12947-15133</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00802738</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>114-3140840-2805024</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>15-12928-93200</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1ZA5T3520301443287</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>112-0163782-4789872</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>18-12925-65132</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>1Z3024W20300799170</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>114-4592665-1282659</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14-12930-44483</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01446875</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>113-6596600-2407435</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>10-12935-74847</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33419534</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>111-0287793-5740220</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>19-12924-17640</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01447463</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>113-4054909-3593014</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>26-12915-31709</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>1ZA5T3520301443241</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>113-9429656-1739405</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>08-12938-69957</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00806645</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>112-7517354-7596220</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>19-12924-40995</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01448944</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>113-1204470-2667418</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>19-12924-16048</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>1ZA5T352YW01446740</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>114-3974135-4995407</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>27-12914-97960</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00804941</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>114-9444413-5227407</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>704067812</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>1Z3024W20300803682</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>112-6419306-5168246</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>25-12917-96224</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00806243</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>113-9205704-4961051</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>10-12936-21810</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>1Z3024W2YW00805842</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>113-2299668-6301016</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>25-12918-29177</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33426768</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>111-4714273-6097824</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>703999666</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33415234</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>112-0513920-0415415</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>08-12938-29265</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>1Z8126VRYW33421656</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>112-3978083-8357811</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>704073723</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>1Z3024W20300806769</t>
         </is>
       </c>
     </row>

</xml_diff>